<commit_message>
changed data use, iter vs rec
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/data/Book4.xlsx
+++ b/REyeker-DataAnalyses-Python/data/Book4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\REyeker\REyeker-DataAnalyses-Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE27CD61-EE6A-4AF6-962B-E17521F8B1AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E013AAD-5468-415B-88C0-6C7841CA6542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>TR20_01</t>
   </si>
@@ -574,6 +574,96 @@
   </si>
   <si>
     <t xml:space="preserve">101-25 315-29 266-11 136-73 410-76 168-107 209-28 196-105 314-84 190-126 382-121 499-141 277-218 405-210 228-278 333-307 612-309 763-317 532-301 719-294 384-284 343-206 187-233 390-208 453-148 488-84 478-126 273-100 292-208 357-228 231-251 249-315 367-294 693-302 248-234 722-309 251-272 688-316 289-259 456-291 355-127 282-90 381-123 </t>
+  </si>
+  <si>
+    <t>TI20_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470-71 128-9 213-54 416-63 202-127 279-133 549-131 139-204 307-204 522-211 202-252 362-249 189-296 289-216 220-299 182-331 365-335 226-361 225-283 235-244 279-341 345-274 273-379 225-382 211-436 153-492 161-265 202-200 353-280 431-228 465-326 181-465 329-104 276-421 449-234 383-166 331-116 642-117 243-118 275-267 272-322 234-254 245-286 237-335 411-330 261-353 244-350 235-250 242-352 274-253 238-417 239-297 264-259 267-365 244-414 244-263 248-421 200-325 261-297 241-244 236-368 272-263 262-363 225-393 251-281 329-243 243-370 240-414 273-295 369-245 247-344 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">186-34 459-121 202-112 227-220 465-239 230-288 405-340 252-390 362-337 269-118 248-367 208-482 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">247-17 250-64 564-67 248-111 544-146 246-216 250-264 448-220 159-223 185-276 223-109 502-218 213-231 229-271 239-304 501-331 216-362 214-431 186-478 208-404 224-388 268-340 250-245 240-342 228-390 162-456 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">136-13 219-79 494-86 241-100 304-152 581-127 361-216 150-249 251-312 504-334 269-95 388-214 262-274 283-323 245-386 220-465 284-85 522-82 248-104 298-127 538-127 234-108 563-137 384-214 229-267 273-324 234-383 218-248 243-415 266-332 242-390 223-456 227-103 586-130 336-214 252-269 276-341 232-387 282-327 284-357 233-374 209-414 214-457 253-373 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">137-28 210-93 495-100 279-144 219-101 602-148 445-77 316-207 245-276 274-328 258-380 249-416 225-462 224-361 233-402 220-345 300-384 308-318 237-434 272-289 439-174 365-83 280-137 671-145 431-169 188-187 201-243 416-230 526-218 281-268 209-251 209-294 248-405 276-338 365-304 527-330 255-403 214-244 370-111 175-75 490-172 175-154 221-293 217-253 214-411 221-479 277-353 146-254 339-300 250-404 92-465 181-162 141-97 532-166 538-138 356-345 290-448 305-262 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">394-72 376-103 390-136 457-120 323-258 300-305 321-335 288-374 273-411 292-350 297-276 398-143 256-95 631-126 332-260 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">216-56 408-83 180-75 178-116 336-140 454-137 222-69 224-107 172-15 278-150 518-163 335-227 281-266 235-294 452-328 262-371 269-274 222-203 245-86 260-123 526-60 237-123 506-136 261-128 493-135 334-248 262-304 215-252 239-297 259-326 397-342 243-394 230-293 251-400 220-451 299-368 336-340 260-393 341-322 250-242 236-399 236-348 228-382 318-328 236-400 173-456 228-404 293-306 244-383 320-333 217-247 228-369 256-236 224-353 250-401 250-364 225-393 220-416 244-360 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">107-3 323-18 160-65 478-77 234-110 555-130 256-130 222-216 262-143 257-68 482-63 299-95 274-130 573-140 495-212 205-213 497-220 509-121 491-199 260-252 231-300 261-266 265-310 466-332 264-339 257-387 257-320 217-421 217-466 251-404 247-349 245-315 243-385 271-333 236-272 222-242 436-227 306-217 220-267 230-227 478-214 200-230 245-271 282-320 261-246 253-271 259-299 498-332 269-334 489-338 256-332 296-364 281-328 274-263 315-335 292-365 259-398 304-344 270-282 284-361 296-318 286-286 279-256 271-279 279-253 278-304 273-332 256-294 266-243 264-290 272-328 210-385 228-462 238-393 258-341 198-421 244-385 270-347 247-395 245-422 277-332 253-290 249-263 332-222 446-326 236-134 555-147 387-134 191-462 258-144 250-97 236-336 499-333 250-332 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">130-25 446-83 357-135 327-227 264-302 286-363 256-412 251-369 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">94-35 308-32 382-36 351-91 125-100 336-82 74-81 327-93 109-88 456-86 148-122 420-146 656-136 373-128 663-135 344-133 186-120 485-131 159-233 456-227 192-227 242-251 440-210 116-224 373-216 332-217 284-219 325-213 306-211 298-211 298-211 530-116 232-119 253-230 521-215 205-224 424-202 222-259 225-305 236-258 230-313 226-270 230-315 240-268 219-307 245-308 228-248 214-302 371-315 221-272 378-238 165-233 228-268 210-306 220-276 323-237 245-323 243-369 500-314 236-320 417-317 272-320 578-105 298-94 236-364 228-336 233-281 226-319 534-334 303-338 238-374 444-326 268-295 240-257 325-335 260-376 330-341 223-254 230-322 462-336 226-341 223-362 170-450 50-495 38-522 292-400 228-393 232-352 210-250 233-330 238-379 233-280 380-218 129-275 258-312 454-216 362-346 251-380 245-268 248-330 235-378 202-456 244-400 235-320 457-332 214-319 488-330 254-365 245-299 249-270 218-140 213-55 447-72 574-120 269-124 175-88 197-126 242-274 258-335 220-264 363-346 220-268 406-244 219-262 361-320 268-348 238-364 250-392 148-139 268-91 472-112 270-112 278-79 540-107 569-80 576-119 299-133 556-129 213-144 294-186 281-225 255-279 251-279 270-328 249-381 236-330 225-379 263-337 236-400 254-363 293-314 204-384 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">119-43 325-24 158-117 221-94 250-76 274-76 302-76 319-76 531-77 134-169 185-133 443-120 111-230 363-201 128-288 249-309 234-358 221-421 196-487 184-53 251-90 299-122 318-162 216-194 455-222 170-253 164-230 569-192 150-272 140-256 154-314 174-366 293-302 367-306 472-332 288-347 234-400 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100-7 276-84 574-80 249-127 528-134 256-139 219-212 486-226 281-265 270-325 515-330 232-368 232-414 225-470 282-340 302-266 390-227 588-89 246-109 328-109 619-126 252-111 217-250 493-221 256-266 264-356 496-333 230-385 176-222 221-376 273-252 247-360 245-415 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">56-26 262-37 159-93 419-133 173-220 429-216 234-240 452-225 256-287 243-339 480-325 258-333 225-466 252-390 226-271 436-331 218-271 250-337 241-98 608-140 444-217 432-317 223-362 273-243 245-358 211-422 245-358 227-458 249-360 250-393 393-331 246-368 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">248-112 385-78 411-116 212-230 216-324 464-341 222-374 184-459 244-343 244-177 320-128 532-140 241-284 304-88 289-237 264-306 237-378 265-240 433-221 234-257 240-292 479-202 290-333 256-365 216-430 192-454 249-361 390-330 288-327 275-360 298-263 251-349 256-274 220-389 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">83-28 262-26 194-98 436-88 234-125 508-131 274-114 197-235 414-228 207-268 265-308 519-332 231-367 280-248 261-371 238-416 289-253 237-424 223-478 225-349 245-422 225-464 263-369 258-414 294-355 223-404 187-252 204-362 182-454 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">127-9 283-65 546-63 215-109 511-129 255-211 498-221 207-266 222-246 477-225 233-293 227-257 250-299 267-235 261-328 518-333 215-407 268-299 245-376 295-333 242-385 260-342 259-315 261-280 244-400 252-367 253-263 240-400 299-347 249-381 250-402 231-452 241-384 310-324 623-123 479-93 277-72 229-91 561-131 346-276 409-365 392-332 250-390 279-315 253-388 260-369 232-454 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">127-22 225-91 513-87 229-117 513-76 219-91 539-134 305-236 239-119 671-162 428-219 255-257 255-301 299-338 249-383 329-329 247-372 227-465 217-386 239-489 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">168-58 252-178 369-112 577-130 351-108 521-146 356-241 238-267 268-325 267-290 500-213 255-325 228-295 263-329 278-364 267-273 267-364 259-265 246-394 273-396 300-338 482-228 515-97 484-124 267-108 453-218 186-277 444-348 306-339 231-392 259-354 244-418 231-474 431-154 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">151-28 193-83 457-81 205-115 503-133 239-213 467-213 213-254 205-279 239-305 407-331 235-377 227-422 228-343 257-330 197-229 492-227 243-255 223-224 485-217 209-247 221-281 245-311 511-331 233-351 215-407 231-368 189-453 212-386 252-344 255-303 257-329 448-237 271-255 325-246 496-197 491-215 567-132 319-137 319-207 504-138 263-102 531-63 580-129 239-133 347-205 182-254 213-327 473-328 231-365 265-255 243-351 225-407 219-352 233-425 185-480 211-403 217-350 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">126-20 187-80 492-82 257-134 504-147 219-221 416-216 198-228 201-280 444-200 234-253 233-288 230-252 242-327 409-321 287-320 254-376 206-453 216-421 230-382 239-248 362-226 223-271 300-208 249-264 249-307 278-323 234-354 241-244 388-86 256-124 473-132 220-324 225-351 238-244 236-357 236-377 232-393 228-362 226-384 233-237 224-393 199-452 216-418 225-388 228-368 200-468 216-415 225-378 233-352 243-328 242-350 222-399 230-367 228-294 236-252 271-218 250-237 242-260 243-290 257-333 255-270 257-292 306-336 260-387 246-415 223-457 229-412 246-352 229-351 258-333 228-403 232-384 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">418-135 372-326 269-394 294-124 309-226 276-313 259-26 446-90 637-142 310-224 234-290 281-347 235-395 220-461 208-310 281-113 596-127 289-214 214-281 297-336 240-358 195-392 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">69-36 300-36 149-92 299-96 511-81 199-120 409-127 580-125 220-134 366-128 473-126 282-119 625-122 277-111 568-143 287-222 482-212 234-238 227-280 298-260 244-309 317-263 251-315 515-216 600-117 217-22 234-127 676-162 378-232 257-291 237-329 277-264 317-244 305-344 426-327 294-352 271-251 283-364 252-384 290-343 306-250 269-368 280-266 242-382 250-247 229-401 270-307 267-344 377-327 279-364 232-390 216-459 266-406 270-355 318-337 186-457 300-155 468-147 556-136 264-165 205-132 262-412 243-466 257-144 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">119-104 233-9 255-50 167-85 517-62 227-107 190-119 529-127 649-138 169-92 176-266 282-199 448-225 169-240 308-241 206-219 338-230 289-205 173-240 313-248 498-234 43-251 307-234 298-252 202-275 209-317 535-318 187-399 211-360 176-438 180-482 392-52 373-120 212-102 305-154 615-147 178-105 180-224 511-204 240-401 438-229 165-241 353-246 149-269 232-298 258-321 238-372 240-418 208-474 352-321 177-308 143-318 311-329 429-325 482-330 381-335 259-254 269-327 426-335 245-299 245-235 232-346 397-331 455-332 189-338 216-354 205-405 219-372 156-512 205-455 187-342 242-314 485-321 271-338 226-350 340-214 222-266 345-250 219-338 210-384 257-250 202-382 243-237 221-392 212-401 215-341 262-142 251-251 193-515 231-400 207-467 195-464 191-396 157-318 307-331 260-359 235-391 237-375 288-354 256-311 237-257 236-338 201-384 209-360 303-361 225-291 239-342 209-377 230-259 276-251 232-372 195-394 173-490 172-194 396-202 362-426 189-481 348-147 568-134 223-399 235-349 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">149-20 129-80 313-78 109-83 475-88 208-115 467-123 193-137 180-216 128-229 220-219 413-224 270-251 151-260 190-286 208-271 236-248 476-224 187-244 273-301 194-253 263-301 243-328 428-339 377-340 235-361 216-379 240-283 248-251 245-366 228-390 264-347 230-404 166-424 164-471 191-403 198-350 196-288 183-255 188-229 220-150 589-136 315-71 264-101 177-254 206-231 283-305 250-365 217-423 196-498 55-510 220-253 187-98 450-107 641-128 234-119 399-137 581-128 246-198 494-202 258-254 266-280 271-260 227-343 259-272 322-228 249-260 264-301 258-334 425-329 235-345 502-320 268-316 302-268 309-254 353-311 603-172 332-371 374-340 277-296 239-268 217-294 253-237 245-369 251-360 233-253 258-394 205-427 206-464 247-386 248-359 237-386 307-268 440-221 440-317 274-289 279-246 228-428 245-396 265-361 226-245 288-317 264-353 222-387 205-366 239-391 222-461 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">89-13 170-69 307-15 305-66 508-77 182-107 438-138 306-204 154-220 460-213 234-254 194-281 217-332 146-77 121-32 134-63 112-11 211-97 373-68 225-81 496-70 581-76 581-76 581-76 581-76 124-86 432-85 154-99 229-125 458-131 352-69 227-21 206-98 248-234 263-80 245-277 242-301 235-330 232-354 229-374 229-411 232-338 230-433 199-468 318-349 248-403 286-311 474-226 328-242 318-342 245-234 247-272 271-308 472-317 275-366 282-266 271-364 286-244 259-363 237-381 239-244 223-468 233-382 261-246 228-423 241-374 272-331 258-247 267-270 244-115 478-73 511-107 333-239 248-282 267-325 244-366 229-480 275-396 275-332 289-284 284-335 264-259 263-294 263-348 251-370 282-295 245-385 211-471 263-376 240-422 287-340 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">67-23 220-68 442-81 174-101 300-138 588-118 243-206 483-207 187-247 323-244 374-134 402-230 144-239 403-244 182-272 171-331 390-331 205-375 208-409 210-347 216-387 237-353 256-237 247-359 247-417 226-467 464-417 159-464 164-240 476-204 162-250 227-293 264-328 376-274 290-372 236-30 150-156 174-99 248-462 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">87-22 232-75 477-79 208-93 276-132 464-140 192-214 437-217 263-250 234-297 256-331 507-331 246-358 250-411 152-318 411-325 240-357 239-420 234-474 248-404 245-348 523-321 608-129 346-325 223-475 637-105 238-115 229-252 253-298 280-336 248-391 237-478 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">244-22 268-99 371-196 368-123 627-134 247-108 337-239 291-326 272-403 247-467 265-410 257-355 256-285 279-227 329-339 275-302 277-230 270-139 295-277 297-395 156-229 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -610,8 +700,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -896,168 +991,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="80.86328125" customWidth="1"/>
+    <col min="1" max="1" width="32.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="B19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="B21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>